<commit_message>
ya faltaria analizar glosas y validar algunas cosas
</commit_message>
<xml_diff>
--- a/Clasificador.xlsx
+++ b/Clasificador.xlsx
@@ -2,19 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rserdan\Desktop\Desarrollo Cambiaria\AppCambiaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
+    <sheet name="Clasificador" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="33" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="232">
   <si>
     <t>Balanza Cambiaria</t>
   </si>
@@ -741,6 +745,18 @@
   </si>
   <si>
     <t>7164, 7954, 5968</t>
+  </si>
+  <si>
+    <t>Detalle 1</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>todas</t>
   </si>
 </sst>
 </file>
@@ -823,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -835,6 +851,28 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,6 +888,1034 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Serdan Wilder" refreshedDate="44600.448242361112" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="69">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:H70" sheet="Clasificador"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Nivel 2" numFmtId="0">
+      <sharedItems count="2">
+        <s v="I. INGRESO DE DIVISAS"/>
+        <s v="II. EGRESO DE DIVISAS"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nivel 3" numFmtId="0">
+      <sharedItems count="20">
+        <s v="I.A. POR EXPORTACIONES"/>
+        <s v="I.B. RENTA"/>
+        <s v="I.C. DONACIONES"/>
+        <s v="I.D. BANCOS-CHEQUES"/>
+        <s v="I.E. DESEMBOLSOS DEUDA EXTERNA"/>
+        <s v="I.F. REC. ACREENCIAS BIDESA"/>
+        <s v="I.G.CEDES"/>
+        <s v="I.H. LETRAS DE TESORERÍA (LT's)"/>
+        <s v="I.J REMESAS FAMILIARES"/>
+        <s v="I.K. OTROS"/>
+        <s v="II.A POR IMPORTACION"/>
+        <s v="II.B SERVICIO DE DEUDA EXTERNA"/>
+        <s v="II.C. SECTOR PRIVADO-BANCOS"/>
+        <s v="II.D. PRESTAMOS AL SISTEMA BANCARIO"/>
+        <s v="II.E. CEDES"/>
+        <s v="II.F. LETRAS DE TESORERIA (LT's)"/>
+        <s v="II.G. OTROS"/>
+        <s v="IV. F.M.I. - Capital"/>
+        <s v="V. F.M.I. - Intereses"/>
+        <s v="II.J YPFB Costos Recuperables y Retribuciones a Empresas"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nivel 4" numFmtId="0">
+      <sharedItems count="36">
+        <s v="I.A.1. DE BIENES"/>
+        <s v="I.A.2 DE SERVICIOS"/>
+        <s v="RENTA"/>
+        <s v="DONACIONES"/>
+        <s v="ENCAJE LEGAL"/>
+        <s v="FONDOS EN CUSTODIA "/>
+        <s v="CUENTA CORRIENTE (3)"/>
+        <s v="TRANSFERENCIAS"/>
+        <s v="OTROS"/>
+        <s v="RAL"/>
+        <s v="TRANSFERENCIAS del EXT."/>
+        <s v="MEDIANO Y LARGO PLAZO"/>
+        <s v="CORTO PLAZO"/>
+        <s v="REC. ACREENCIAS BIDESA"/>
+        <s v="CEDES"/>
+        <s v="LETRAS DE TESORERÍA (LT's)"/>
+        <s v="REMESAS FAMILIARES"/>
+        <s v="CUENTAS DE ORGANISMOS INTERNACIONALES "/>
+        <s v="ABONOS TRANSITORIOS "/>
+        <s v="AJUSTE POR ARBITRAJE DE SALDOS "/>
+        <s v="OTROS PORTAFOLIOS"/>
+        <s v="EXTRACONTABLES"/>
+        <s v="FMI-ESAF"/>
+        <s v="II.A.1 DE BIENES"/>
+        <s v="II.A.2 DE SERVICIOS CORRIENTES"/>
+        <s v="MEDIANO Y LARGO PLAZO "/>
+        <s v="RETIRO ENCAJE LEGAL"/>
+        <s v="OPERACIONES BANCARIAS (3)"/>
+        <s v="TRANSFERENCIAS al EXT."/>
+        <s v="BOLSIN"/>
+        <s v="PRESTAMOS AL SISTEMA BANCARIO"/>
+        <s v="LETRAS DE TESORERIA (LT's)"/>
+        <s v="AJUSTE POR ARBITRAJE DE SALDOS"/>
+        <s v="F.M.I. - Capital"/>
+        <s v="F.M.I. - Intereses"/>
+        <s v="YPFB Costos Recuperables y Retribuciones a Empresas"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nivel 5 " numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Nivel  6" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Clasificación" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Detalle 1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="69">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="ENAF-COMIBOL"/>
+    <s v="ENAF-COMIBOL (BCI1)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="Y.P.F.B. Libre Dispon."/>
+    <s v="Y.P.F.B. Libre Dispon. (BCI2)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="Y.P.F.B. Otros"/>
+    <s v="Y.P.F.B. Argentina (BCI3)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="Y.P.F.B. Otros"/>
+    <s v="Y.P.F.B. Brasil (BCI4)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="Y.P.F.B. Otros"/>
+    <s v="Y.P.F.B. Otros (BCI5)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="VINTO"/>
+    <s v="VINTO (BCI6)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="OTRAS EMPRESAS"/>
+    <s v="OTRAS EMPRESAS (BCI7)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PRIVADO"/>
+    <s v="MINERIA MEDIANA"/>
+    <s v="MINERIA MEDIANA (BCI8)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PRIVADO"/>
+    <s v="AGROPECUARIOS"/>
+    <s v="AGROPECUARIOS (BCI9)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="SECTOR PRIVADO"/>
+    <s v="OTROS"/>
+    <s v="OTROS (BCI10)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="CONVENIO DE CRED. RECIP (1)"/>
+    <s v="CONVENIO DE CRED. RECIP (1)"/>
+    <s v="CONVENIO DE CRED. RECIP (1) (BCI11)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="CORRIENTES"/>
+    <s v="CORRIENTES"/>
+    <s v="CORRIENTES (BCI12)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="FINANCIEROS"/>
+    <s v="FINANCIEROS"/>
+    <s v="FINANCIEROS (BCI13)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="RENTA"/>
+    <s v="RENTA"/>
+    <s v="RENTA (BCI14)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="DONACIONES"/>
+    <s v="DONACIONES"/>
+    <s v="DONACIONES (BCI15)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="4"/>
+    <s v="ENCAJE LEGAL"/>
+    <s v="ENCAJE LEGAL"/>
+    <s v="ENCAJE LEGAL (BCI16)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="5"/>
+    <s v="FONDOS EN CUSTODIA "/>
+    <s v="FONDOS EN CUSTODIA "/>
+    <s v="FONDOS EN CUSTODIA (BCI17)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="6"/>
+    <s v="CUENTA CORRIENTE (3)"/>
+    <s v="CUENTA CORRIENTE (3)"/>
+    <s v="CUENTA CORRIENTE (3) (BCI18)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="7"/>
+    <s v="TRANSFERENCIAS"/>
+    <s v="TRANSFERENCIAS"/>
+    <s v="TRANSFERENCIAS (BCI19)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="8"/>
+    <s v="OTROS"/>
+    <s v="OTROS"/>
+    <s v="OTROS (BCI20)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="9"/>
+    <s v="RAL"/>
+    <s v="RAL"/>
+    <s v="RAL (BCI21)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="10"/>
+    <s v="TRANSFERENCIAS del EXT."/>
+    <s v="TRANSFERENCIAS del EXT."/>
+    <s v="TRANSFERENCIAS del EXT. (BCI22)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="11"/>
+    <s v="SPNF"/>
+    <s v="SPNF"/>
+    <s v="SPNF (BCI23)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="11"/>
+    <s v="BCB"/>
+    <s v="BCB"/>
+    <s v="BCB (BCI24)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="12"/>
+    <s v="CORTO PLAZO"/>
+    <s v="CORTO PLAZO"/>
+    <s v="CORTO PLAZO (BCI25)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="13"/>
+    <s v="REC. ACREENCIAS BIDESA"/>
+    <s v="REC. ACREENCIAS BIDESA"/>
+    <s v="REC. ACREENCIAS BIDESA (BCI26)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="14"/>
+    <s v="CEDES"/>
+    <s v="CEDES"/>
+    <s v="CEDES (BCI27)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="15"/>
+    <s v="LETRAS DE TESORERÍA (LT's)"/>
+    <s v="LETRAS DE TESORERÍA (LT's)"/>
+    <s v="LETRAS DE TESORERÍA (LT's) (BCI28)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="16"/>
+    <s v="REMESAS FAMILIARES"/>
+    <s v="REMESAS FAMILIARES"/>
+    <s v="REMESAS FAMILIARES (BCI29)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="17"/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES "/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES "/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES (BCI30)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="18"/>
+    <s v="ABONOS TRANSITORIOS "/>
+    <s v="ABONOS TRANSITORIOS "/>
+    <s v="ABONOS TRANSITORIOS (BCI31)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="19"/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS "/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS "/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS (BCI32)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="20"/>
+    <s v="OTROS PORTAFOLIOS"/>
+    <s v="OTROS PORTAFOLIOS"/>
+    <s v="OTROS PORTAFOLIOS (BCI33)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="21"/>
+    <s v="EXTRACONTABLES"/>
+    <s v="EXTRACONTABLES"/>
+    <s v="EXTRACONTABLES (BCI34)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="22"/>
+    <s v="FMI-ESAF"/>
+    <s v="FMI-ESAF"/>
+    <s v="FMI-ESAF (BCI35)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="COMIBOL-ENAF"/>
+    <s v="COMIBOL-ENAF (BCE1)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="Y.P.F.B."/>
+    <s v="Y.P.F.B. (BCE2)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="BAMIN"/>
+    <s v="BAMIN (BCE3)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="SECTOR PUBLICO"/>
+    <s v="OTRAS EMPRESAS"/>
+    <s v="OTRAS EMPRESAS (BCE4)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="BOLSIN SEC. PUBLICO"/>
+    <s v="BOLSIN SEC. PUBLICO"/>
+    <s v="BOLSIN SEC. PUBLICO (BCE5)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="23"/>
+    <s v="CONVENIO CRED. RECIP.(1),(2)"/>
+    <s v="CONVENIO CRED. RECIP.(1),(2)"/>
+    <s v="CONVENIO CRED. RECIP.(1),(2) (BCE6)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="HABERES"/>
+    <s v="HABERES"/>
+    <s v="HABERES (BCE7)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="VIATICOS"/>
+    <s v="VIATICOS"/>
+    <s v="VIATICOS (BCE8)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="SERVICIO TECNICO"/>
+    <s v="SERVICIO TECNICO"/>
+    <s v="SERVICIO TECNICO (BCE9)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="FLETES Y TRANSPORTES"/>
+    <s v="FLETES Y TRANSPORTES"/>
+    <s v="FLETES Y TRANSPORTES (BCE10)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="CUOTA A ORG. INTERNAC."/>
+    <s v="CUOTA A ORG. INTERNAC."/>
+    <s v="CUOTA A ORG. INTERNAC. (BCE11)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="24"/>
+    <s v="OTROS"/>
+    <s v="OTROS"/>
+    <s v="OTROS (BCE12)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="25"/>
+    <s v="II.B.1. CAPITAL"/>
+    <s v="CAPITAL"/>
+    <s v="CAPITAL (BCE13)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="25"/>
+    <s v="II.B.2. INTERESES"/>
+    <s v="INTERESES"/>
+    <s v="INTERESES (BCE14)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="12"/>
+    <s v="II.B.1. CAPITAL"/>
+    <s v="CAPITAL"/>
+    <s v="CAPITAL (BCE15)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="12"/>
+    <s v="II.B.2. INTERESES"/>
+    <s v="INTERESES"/>
+    <s v="INTERESES (BCE16)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="26"/>
+    <s v="RETIRO ENCAJE LEGAL"/>
+    <s v="RETIRO ENCAJE LEGAL"/>
+    <s v="RETIRO ENCAJE LEGAL (BCE17)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="5"/>
+    <s v="FONDOS EN CUSTODIA "/>
+    <s v="FONDOS EN CUSTODIA "/>
+    <s v="FONDOS EN CUSTODIA (BCE18)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="27"/>
+    <s v="OPERACIONES BANCARIAS (3)"/>
+    <s v="OPERACIONES BANCARIAS (3)"/>
+    <s v="OPERACIONES BANCARIAS (3) (BCE19)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="8"/>
+    <s v="OTROS"/>
+    <s v="OTROS"/>
+    <s v="OTROS (BCE20)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="9"/>
+    <s v="RAL"/>
+    <s v="RAL"/>
+    <s v="RAL (BCE21)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="28"/>
+    <s v="TRANSFERENCIAS al EXT."/>
+    <s v="TRANSFERENCIAS al EXT."/>
+    <s v="TRANSFERENCIAS al EXT. (BCE22)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="29"/>
+    <s v="BOLSIN"/>
+    <s v="BOLSIN"/>
+    <s v="BOLSIN (BCE23)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="30"/>
+    <s v="PRESTAMOS AL SISTEMA BANCARIO"/>
+    <s v="PRESTAMOS AL SISTEMA BANCARIO"/>
+    <s v="PRESTAMOS AL SISTEMA BANCARIO (BCE24)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="14"/>
+    <x v="14"/>
+    <s v="CEDES"/>
+    <s v="CEDES"/>
+    <s v="CEDES (BCE25)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="15"/>
+    <x v="31"/>
+    <s v="LETRAS DE TESORERIA (LT's)"/>
+    <s v="LETRAS DE TESORERIA (LT's)"/>
+    <s v="LETRAS DE TESORERIA (LT's) (BCE26)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="17"/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES "/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES "/>
+    <s v="CUENTAS DE ORGANISMOS INTERNACIONALES (BCE27)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="18"/>
+    <s v="ABONOS TRANSITORIOS "/>
+    <s v="ABONOS TRANSITORIOS "/>
+    <s v="ABONOS TRANSITORIOS (BCE28)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="32"/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS"/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS"/>
+    <s v="AJUSTE POR ARBITRAJE DE SALDOS (BCE29)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="20"/>
+    <s v="OTROS PORTAFOLIOS"/>
+    <s v="OTROS PORTAFOLIOS"/>
+    <s v="OTROS PORTAFOLIOS (BCE30)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="21"/>
+    <s v="EXTRACONTABLES"/>
+    <s v="EXTRACONTABLES"/>
+    <s v="EXTRACONTABLES (BCE31)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="17"/>
+    <x v="33"/>
+    <s v="F.M.I. - Capital"/>
+    <s v="F.M.I. - Capital"/>
+    <s v="F.M.I. - Capital (BCE32)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="18"/>
+    <x v="34"/>
+    <s v="F.M.I. - Intereses"/>
+    <s v="F.M.I. - Intereses"/>
+    <s v="F.M.I. - Intereses (BCE33)"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="19"/>
+    <x v="35"/>
+    <s v="YPFB Costos Recuperables y Retribuciones a Empresas"/>
+    <s v="YPFB Costos Recuperables y Retribuciones a Empresas"/>
+    <s v="YPFB Costos Recuperables y Retribuciones a Empresas (BCE34)"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="21">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="19"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="37">
+        <item x="18"/>
+        <item x="32"/>
+        <item x="19"/>
+        <item x="29"/>
+        <item x="14"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="22"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="31"/>
+        <item x="15"/>
+        <item x="11"/>
+        <item x="25"/>
+        <item x="27"/>
+        <item x="8"/>
+        <item x="20"/>
+        <item x="30"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="16"/>
+        <item x="2"/>
+        <item x="26"/>
+        <item x="7"/>
+        <item x="28"/>
+        <item x="10"/>
+        <item x="35"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="68">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1115,13 +2181,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A3:A71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:O70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,14 +2561,15 @@
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
-    <col min="12" max="12" width="43.85546875" customWidth="1"/>
+    <col min="7" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.140625" customWidth="1"/>
+    <col min="13" max="13" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1160,26 +2591,29 @@
       <c r="G1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1201,20 +2635,21 @@
       <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="H2" s="4"/>
+      <c r="K2" s="10">
         <v>412</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>818</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>204</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1259,23 +2694,24 @@
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J4">
+      <c r="H4" s="4"/>
+      <c r="K4" s="10">
         <v>404</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>5968</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>200</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>12</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1297,20 +2733,21 @@
       <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J5">
+      <c r="H5" s="4"/>
+      <c r="K5" s="10">
         <v>404</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>5968</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>200</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1332,20 +2769,21 @@
       <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J6">
+      <c r="H6" s="4"/>
+      <c r="K6" s="10">
         <v>404</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>227</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>201</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1367,17 +2805,18 @@
       <c r="G7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J7">
+      <c r="H7" s="4"/>
+      <c r="K7" s="10">
         <v>404</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>6215</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1399,17 +2838,18 @@
       <c r="G8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J8">
+      <c r="H8" s="8"/>
+      <c r="K8" s="10">
         <v>412</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>818</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +2872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +2895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1477,11 +2917,11 @@
       <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1503,11 +2943,11 @@
       <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1529,20 +2969,21 @@
       <c r="G13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="H13" s="4"/>
+      <c r="K13" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L13" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="M13" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +3006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1587,20 +3028,21 @@
       <c r="G15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="H15" s="4"/>
+      <c r="K15" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>213</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1622,20 +3064,21 @@
       <c r="G16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J16">
+      <c r="H16" s="4"/>
+      <c r="K16" s="10">
         <v>406</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>8263</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>222</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1657,11 +3100,11 @@
       <c r="G17" t="s">
         <v>49</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +3127,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -1706,20 +3149,20 @@
       <c r="G19" t="s">
         <v>54</v>
       </c>
-      <c r="J19">
+      <c r="K19" s="10">
         <v>828</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>3500</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>221</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1742,7 +3185,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1765,7 +3208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1787,11 +3230,11 @@
       <c r="G22" t="s">
         <v>60</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1813,20 +3256,21 @@
       <c r="G23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="H23" s="4"/>
+      <c r="K23" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="M23" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1848,11 +3292,11 @@
       <c r="G24" t="s">
         <v>67</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1874,11 +3318,11 @@
       <c r="G25" t="s">
         <v>70</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1900,11 +3344,11 @@
       <c r="G26" t="s">
         <v>72</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +3371,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +3394,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +3417,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -1995,11 +3439,11 @@
       <c r="G30" t="s">
         <v>84</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2021,11 +3465,11 @@
       <c r="G31" t="s">
         <v>87</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2047,14 +3491,15 @@
       <c r="G32" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J32">
+      <c r="H32" s="4"/>
+      <c r="K32" s="10">
         <v>498</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2076,18 +3521,19 @@
       <c r="G33" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="H33" s="4"/>
+      <c r="I33" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="12"/>
       <c r="L33" s="4"/>
-      <c r="M33" t="s">
+      <c r="M33" s="4"/>
+      <c r="N33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2109,17 +3555,18 @@
       <c r="G34" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="H34" s="4"/>
+      <c r="K34" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="L34" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="M34" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +3589,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2165,7 +3612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
@@ -2187,17 +3634,18 @@
       <c r="G37" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="J37">
+      <c r="H37" s="8"/>
+      <c r="K37" s="10">
         <v>412</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>818</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
@@ -2219,20 +3667,21 @@
       <c r="G38" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J38">
+      <c r="H38" s="4"/>
+      <c r="K38" s="10">
         <v>405</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>3305</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>200</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +3704,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>0</v>
       </c>
@@ -2277,20 +3726,21 @@
       <c r="G40" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="H40" s="4"/>
+      <c r="K40" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="L40" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>200</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +3763,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>0</v>
       </c>
@@ -2335,17 +3785,18 @@
       <c r="G42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J42">
+      <c r="H42" s="4"/>
+      <c r="K42" s="10">
         <v>25</v>
       </c>
-      <c r="K42">
-        <v>166</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="L42" t="s">
+        <v>231</v>
+      </c>
+      <c r="N42" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>0</v>
       </c>
@@ -2367,11 +3818,11 @@
       <c r="G43" t="s">
         <v>120</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>0</v>
       </c>
@@ -2394,7 +3845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>0</v>
       </c>
@@ -2416,11 +3867,11 @@
       <c r="G45" t="s">
         <v>125</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>0</v>
       </c>
@@ -2442,20 +3893,21 @@
       <c r="G46" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="J46">
+      <c r="H46" s="4"/>
+      <c r="K46" s="10">
         <v>412</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>3987</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>200</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>0</v>
       </c>
@@ -2478,7 +3930,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>0</v>
       </c>
@@ -2500,20 +3952,21 @@
       <c r="G48" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="H48" s="4"/>
+      <c r="K48" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="L48" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>200</v>
       </c>
-      <c r="M48" t="s">
+      <c r="N48" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -2535,20 +3988,20 @@
       <c r="G49" t="s">
         <v>138</v>
       </c>
-      <c r="J49">
+      <c r="K49" s="10">
         <v>412</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>818</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>214</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>0</v>
       </c>
@@ -2570,20 +4023,20 @@
       <c r="G50" t="s">
         <v>142</v>
       </c>
-      <c r="J50">
+      <c r="K50" s="10">
         <v>412</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>818</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>214</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>0</v>
       </c>
@@ -2605,11 +4058,11 @@
       <c r="G51" t="s">
         <v>143</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>0</v>
       </c>
@@ -2631,11 +4084,11 @@
       <c r="G52" t="s">
         <v>144</v>
       </c>
-      <c r="M52" t="s">
+      <c r="N52" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>0</v>
       </c>
@@ -2657,11 +4110,11 @@
       <c r="G53" t="s">
         <v>147</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>0</v>
       </c>
@@ -2684,7 +4137,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -2706,23 +4159,24 @@
       <c r="G55" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="I55">
+      <c r="H55" s="4"/>
+      <c r="J55">
         <v>7</v>
       </c>
-      <c r="J55">
+      <c r="K55" s="10">
         <v>403</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>220</v>
       </c>
-      <c r="L55" t="s">
+      <c r="M55" t="s">
         <v>202</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>0</v>
       </c>
@@ -2745,7 +4199,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>0</v>
       </c>
@@ -2767,17 +4221,18 @@
       <c r="G57" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="J57">
+      <c r="H57" s="4"/>
+      <c r="K57" s="10">
         <v>403</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>5397</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>0</v>
       </c>
@@ -2799,20 +4254,21 @@
       <c r="G58" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="J58">
+      <c r="H58" s="4"/>
+      <c r="K58" s="10">
         <v>498</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>6817</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>200</v>
       </c>
-      <c r="M58" t="s">
+      <c r="N58" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>0</v>
       </c>
@@ -2835,7 +4291,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +4314,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +4337,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +4360,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>0</v>
       </c>
@@ -2926,11 +4382,11 @@
       <c r="G63" t="s">
         <v>168</v>
       </c>
-      <c r="M63" t="s">
+      <c r="N63" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>0</v>
       </c>
@@ -2952,11 +4408,11 @@
       <c r="G64" t="s">
         <v>170</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>0</v>
       </c>
@@ -2978,18 +4434,18 @@
       <c r="G65" t="s">
         <v>172</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="I65" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="I65" s="4"/>
       <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
+      <c r="K65" s="12"/>
       <c r="L65" s="4"/>
-      <c r="M65" t="s">
+      <c r="M65" s="4"/>
+      <c r="N65" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +4468,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>0</v>
       </c>
@@ -3035,7 +4491,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>0</v>
       </c>
@@ -3058,7 +4514,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +4537,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>0</v>
       </c>
@@ -3103,7 +4559,7 @@
       <c r="G70" t="s">
         <v>183</v>
       </c>
-      <c r="M70" t="s">
+      <c r="N70" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>